<commit_message>
Update the docs about user collection
</commit_message>
<xml_diff>
--- a/docs/Database Structure.xlsx
+++ b/docs/Database Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\OneDrive\Desktop\PROGETTI\HermesChat\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65B29F7-E0BE-4675-BC74-7A0420DB09FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5EE4ED-2B82-4D29-94E8-FC0F9C845D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ED485DD3-099C-4DC2-8130-D198069FC712}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
   <si>
     <t>DB1</t>
   </si>
@@ -210,6 +210,16 @@
   </si>
   <si>
     <t>user</t>
+  </si>
+  <si>
+    <t>ids</t>
+  </si>
+  <si>
+    <t>toAccept</t>
+  </si>
+  <si>
+    <t>id oggetto della
+ collection friendship</t>
   </si>
 </sst>
 </file>
@@ -371,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -430,20 +440,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,11 +787,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C0045A-C665-4A51-9C7A-ABC6AA620FFB}">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -778,17 +806,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="15" t="s">
         <v>17</v>
       </c>
@@ -811,11 +839,11 @@
       <c r="B3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
       <c r="F3" s="10"/>
       <c r="G3" s="17"/>
     </row>
@@ -921,514 +949,515 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="19"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>45</v>
+      </c>
       <c r="G13" s="17"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10"/>
+      <c r="E14" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="27"/>
       <c r="G14" s="17"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="28"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>45</v>
-      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="17"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="19"/>
+      <c r="B17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
       <c r="G17" s="17"/>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="G18" s="17"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
-      <c r="B19" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="10"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="G19" s="17"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="19"/>
       <c r="G20" s="17"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>45</v>
-      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="17"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="17"/>
+      <c r="B22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
       <c r="G22" s="17"/>
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="17"/>
+      <c r="C23" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="G23" s="17"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="13"/>
+      <c r="C24" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="D24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="G24" s="17"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="19"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="17"/>
       <c r="G25" s="17"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="17"/>
       <c r="G26" s="17"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
-      <c r="B27" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="10"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="17"/>
       <c r="G27" s="17"/>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="19"/>
       <c r="G28" s="17"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>45</v>
-      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
       <c r="G29" s="17"/>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30" s="21"/>
-      <c r="F30" s="17"/>
+      <c r="B30" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
       <c r="G30" s="17"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="19"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="G31" s="17"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="16"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="G32" s="17"/>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
-      <c r="B33" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="10"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="20"/>
+      <c r="F33" s="17"/>
       <c r="G33" s="17"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="19"/>
       <c r="G34" s="17"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>45</v>
-      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="16"/>
       <c r="G35" s="17"/>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="17"/>
+      <c r="B36" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="10"/>
       <c r="G36" s="17"/>
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="19"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="G37" s="17"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="19"/>
+    <row r="38" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G38" s="17"/>
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" s="20"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="17"/>
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="10"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="19"/>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
+      <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="17"/>
+      <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="17"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
+      <c r="A44" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="10"/>
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="F45" s="17"/>
+      <c r="F45" s="2"/>
       <c r="G45" s="17"/>
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="17"/>
+      <c r="B46" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="10"/>
       <c r="G46" s="17"/>
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="22" t="s">
-        <v>24</v>
+      <c r="C47" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F47" s="17" t="s">
-        <v>27</v>
-      </c>
+      <c r="F47" s="17"/>
       <c r="G47" s="17"/>
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="22"/>
+      <c r="C48" s="21"/>
       <c r="D48" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E48" s="2"/>
-      <c r="F48" s="17" t="s">
-        <v>28</v>
-      </c>
+      <c r="F48" s="17"/>
       <c r="G48" s="17"/>
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="22"/>
+      <c r="C49" s="21"/>
       <c r="D49" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E49" s="2"/>
-      <c r="F49" s="17" t="s">
-        <v>29</v>
-      </c>
+      <c r="F49" s="17"/>
       <c r="G49" s="17"/>
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="22"/>
+      <c r="C50" s="21" t="s">
+        <v>24</v>
+      </c>
       <c r="D50" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E50" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="F50" s="17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G50" s="17"/>
       <c r="H50" s="2"/>
@@ -1436,25 +1465,27 @@
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="17"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="G51" s="17"/>
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E52" s="2"/>
       <c r="F52" s="17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G52" s="17"/>
       <c r="H52" s="2"/>
@@ -1462,173 +1493,171 @@
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="17"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="G53" s="17"/>
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="C54" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="17"/>
       <c r="G54" s="17"/>
       <c r="H54" s="2"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="17"/>
+      <c r="C55" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="G55" s="17"/>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D56" s="22"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="17" t="s">
-        <v>41</v>
-      </c>
+      <c r="C56" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="17"/>
       <c r="G56" s="17"/>
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="19"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="G57" s="17"/>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="17"/>
       <c r="G58" s="17"/>
       <c r="H58" s="2"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
-      <c r="B59" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="10"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="G59" s="17"/>
       <c r="H59" s="2"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E60" s="2"/>
-      <c r="F60" s="17"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="19"/>
       <c r="G60" s="17"/>
       <c r="H60" s="2"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
-      <c r="B61" s="6"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
       <c r="E61" s="2"/>
-      <c r="F61" s="17"/>
+      <c r="F61" s="2"/>
       <c r="G61" s="17"/>
       <c r="H61" s="2"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" s="17" t="s">
-        <v>27</v>
-      </c>
+      <c r="B62" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="10"/>
       <c r="G62" s="17"/>
       <c r="H62" s="2"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="22"/>
+      <c r="C63" s="21" t="s">
+        <v>20</v>
+      </c>
       <c r="D63" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E63" s="2"/>
-      <c r="F63" s="17" t="s">
-        <v>28</v>
-      </c>
+      <c r="F63" s="17"/>
       <c r="G63" s="17"/>
       <c r="H63" s="2"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="22"/>
+      <c r="C64" s="21"/>
       <c r="D64" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E64" s="2"/>
-      <c r="F64" s="17" t="s">
-        <v>29</v>
-      </c>
+      <c r="F64" s="17"/>
       <c r="G64" s="17"/>
       <c r="H64" s="2"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="22"/>
+      <c r="C65" s="21" t="s">
+        <v>24</v>
+      </c>
       <c r="D65" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E65" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="F65" s="17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G65" s="17"/>
       <c r="H65" s="2"/>
@@ -1636,51 +1665,95 @@
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D66" s="2"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E66" s="2"/>
       <c r="F66" s="17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G66" s="17"/>
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="19"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="2"/>
+      <c r="F67" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="G67" s="17"/>
       <c r="H67" s="2"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="12"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="19"/>
+      <c r="A68" s="6"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E68" s="2"/>
+      <c r="F68" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G68" s="17"/>
       <c r="H68" s="2"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
+      <c r="F69" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G69" s="17"/>
       <c r="H69" s="2"/>
     </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="6"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="12"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="F13:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Db structure and resave Logos
</commit_message>
<xml_diff>
--- a/docs/Database Structure.xlsx
+++ b/docs/Database Structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/deff9de257b50577/Desktop/PROGETTI/HermesChat/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\OneDrive\Desktop\PROGETTI\aaaa\HermesChat\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2A5EE4ED-2B82-4D29-94E8-FC0F9C845D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF94133F-10B6-44FB-8BF0-F948584FFB42}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5215DE-E074-42D4-B2F0-D8790B41234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ED485DD3-099C-4DC2-8130-D198069FC712}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="86">
   <si>
     <t>DB1</t>
   </si>
@@ -215,13 +215,6 @@
     <t>ids</t>
   </si>
   <si>
-    <t>toAccept</t>
-  </si>
-  <si>
-    <t>id oggetto della
- collection friendship</t>
-  </si>
-  <si>
     <t>CALENDARIO</t>
   </si>
   <si>
@@ -266,13 +259,75 @@
   </si>
   <si>
     <t>idUser che ha creato l'evento</t>
+  </si>
+  <si>
+    <t>Vettore contenente gli id delle chat dell'utente</t>
+  </si>
+  <si>
+    <t>Stesso id dell'utente</t>
+  </si>
+  <si>
+    <t>tipo(file,stringa, imagine,sondadggio, grafico)</t>
+  </si>
+  <si>
+    <t>Per i chart e i sondaggi ci sarà un campo 
+chiave options aggiuntivo il quale conterrà</t>
+  </si>
+  <si>
+    <t>CHART</t>
+  </si>
+  <si>
+    <t>grafico a torta:</t>
+  </si>
+  <si>
+    <t>Grafico a barre:</t>
+  </si>
+  <si>
+    <t>SURVEY</t>
+  </si>
+  <si>
+    <t>sondaggio:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> series: vettore di numeri,
+  labels: vettore di stringhe,
+  title: {
+     text: stringa
+  },
+  chart: {
+    height: numero,
+    type: stringa (in questo grafico o è "pie" o "donut")
+  },
+  colors: vettore di stringhe (colori in esadecimale con # incluso)</t>
+  </si>
+  <si>
+    <t>series: [{
+       data: vettore di numeri
+    }],
+  xaxis: { categories: vettore di stringhe},
+  title: {
+     text: stringa
+  },
+  chart: {
+    height: numero,
+    type: stringa (in questo grafico o è "bar" o "line")
+  },
+  colors: vettore di stringhe (colori in esadecimale con # incluso)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"title" -&gt; stringa,
+ "options" :[{
+  "text" -&gt; stringa,
+  "user_voted" -&gt; vettore di stringhe che contiene gli utenti che hanno votato quell'opzione
+     }],
+"exclusion": booleana che indica se i checkbox sono esclusivi o no </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +350,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -304,7 +367,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -423,11 +486,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -486,38 +625,83 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,11 +1017,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C0045A-C665-4A51-9C7A-ABC6AA620FFB}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:O82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44:G82"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -848,7 +1032,12 @@
     <col min="4" max="4" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="11" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="26.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="28.44140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="1"/>
+    <col min="15" max="15" width="25.21875" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -996,46 +1185,36 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>45</v>
-      </c>
+      <c r="D13" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="26"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="24"/>
-      <c r="D14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="30"/>
       <c r="F14" s="26"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="10"/>
       <c r="C15" s="25"/>
-      <c r="D15" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>60</v>
-      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="31"/>
       <c r="F15" s="27"/>
       <c r="G15" s="15"/>
     </row>
@@ -1051,8 +1230,10 @@
       <c r="C17" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="D17" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="21"/>
       <c r="F17" s="8"/>
       <c r="G17" s="15"/>
     </row>
@@ -1111,8 +1292,10 @@
       <c r="C22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="D22" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="21"/>
       <c r="F22" s="8"/>
       <c r="G22" s="15"/>
     </row>
@@ -1199,8 +1382,10 @@
       <c r="C30" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+      <c r="D30" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="21"/>
       <c r="F30" s="8"/>
       <c r="G30" s="15"/>
     </row>
@@ -1234,7 +1419,7 @@
       </c>
       <c r="G32" s="15"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="11"/>
@@ -1245,7 +1430,7 @@
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="10"/>
       <c r="C34" s="3"/>
@@ -1256,12 +1441,12 @@
       <c r="F34" s="17"/>
       <c r="G34" s="15"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="F35" s="14"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="6" t="s">
         <v>54</v>
@@ -1269,12 +1454,14 @@
       <c r="C36" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
+      <c r="D36" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36" s="21"/>
       <c r="F36" s="8"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="11" t="s">
@@ -1287,7 +1474,7 @@
       </c>
       <c r="G37" s="15"/>
     </row>
-    <row r="38" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="11" t="s">
@@ -1304,7 +1491,7 @@
       </c>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="D39" s="1" t="s">
@@ -1314,7 +1501,7 @@
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="10"/>
       <c r="C40" s="2"/>
@@ -1325,7 +1512,7 @@
       <c r="F40" s="17"/>
       <c r="G40" s="15"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="10"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1334,7 +1521,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>13</v>
       </c>
@@ -1347,16 +1534,11 @@
       <c r="F44" s="9"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
       <c r="G45" s="15"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="6" t="s">
         <v>18</v>
@@ -1369,172 +1551,237 @@
       <c r="F46" s="8"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
-      <c r="C47" s="29" t="s">
+      <c r="C47" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D47" s="28" t="s">
+      <c r="D47" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="28" t="s">
+      <c r="E47" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="28" t="s">
+      <c r="C48" s="11"/>
+      <c r="D48" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E48" s="28"/>
       <c r="F48" s="15"/>
       <c r="G48" s="15"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="M48" s="32"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="28" t="s">
+      <c r="C49" s="11"/>
+      <c r="D49" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E49" s="28"/>
       <c r="F49" s="15"/>
       <c r="G49" s="15"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
-      <c r="C50" s="29" t="s">
+      <c r="C50" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="28" t="s">
+      <c r="D50" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F50" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G50" s="15"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F50" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G50" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L50" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="M50" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="N50" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="O50" s="36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="28" t="s">
+      <c r="C51" s="11"/>
+      <c r="D51" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="28"/>
-      <c r="F51" s="15" t="s">
+      <c r="F51" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G51" s="15"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G51" s="38"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="26"/>
+      <c r="L51" s="39"/>
+      <c r="M51" s="39"/>
+      <c r="O51" s="39"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="28" t="s">
+      <c r="C52" s="11"/>
+      <c r="D52" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E52" s="28"/>
-      <c r="F52" s="15" t="s">
+      <c r="F52" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G52" s="15"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G52" s="38"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="26"/>
+      <c r="L52" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="M52" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="N52" s="14"/>
+      <c r="O52" s="40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="28" t="s">
+      <c r="C53" s="11"/>
+      <c r="D53" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E53" s="28"/>
-      <c r="F53" s="15" t="s">
+      <c r="F53" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G53" s="15"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G53" s="41"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="27"/>
+      <c r="L53" s="42"/>
+      <c r="M53" s="40"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="42"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
-      <c r="C54" s="29" t="s">
+      <c r="C54" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="G54" s="43"/>
+      <c r="L54" s="42"/>
+      <c r="M54" s="40"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="42"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
-      <c r="C55" s="29" t="s">
+      <c r="C55" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
       <c r="F55" s="15" t="s">
         <v>34</v>
       </c>
       <c r="G55" s="15"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L55" s="42"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="42"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
-      <c r="C56" s="29" t="s">
+      <c r="C56" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D56" s="29"/>
-      <c r="E56" s="29"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L56" s="42"/>
+      <c r="M56" s="40"/>
+      <c r="N56" s="14"/>
+      <c r="O56" s="42"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
-      <c r="C57" s="29" t="s">
+      <c r="C57" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D57" s="29"/>
-      <c r="E57" s="29"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
       <c r="F57" s="15" t="s">
         <v>37</v>
       </c>
       <c r="G57" s="15"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L57" s="42"/>
+      <c r="M57" s="40"/>
+      <c r="N57" s="14"/>
+      <c r="O57" s="42"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
-      <c r="C58" s="29" t="s">
+      <c r="C58" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
       <c r="F58" s="15"/>
       <c r="G58" s="15"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L58" s="42"/>
+      <c r="M58" s="40"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="42"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
-      <c r="C59" s="29" t="s">
+      <c r="C59" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D59" s="29"/>
-      <c r="E59" s="29"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
       <c r="F59" s="15" t="s">
         <v>41</v>
       </c>
       <c r="G59" s="15"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L59" s="42"/>
+      <c r="M59" s="40"/>
+      <c r="N59" s="14"/>
+      <c r="O59" s="42"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="10"/>
       <c r="C60" s="3" t="s">
@@ -1544,17 +1791,20 @@
       <c r="E60" s="3"/>
       <c r="F60" s="17"/>
       <c r="G60" s="15"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L60" s="42"/>
+      <c r="M60" s="40"/>
+      <c r="N60" s="14"/>
+      <c r="O60" s="42"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
       <c r="G61" s="15"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L61" s="42"/>
+      <c r="M61" s="40"/>
+      <c r="N61" s="14"/>
+      <c r="O61" s="42"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="6" t="s">
         <v>39</v>
@@ -1566,101 +1816,109 @@
       <c r="E62" s="7"/>
       <c r="F62" s="8"/>
       <c r="G62" s="15"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L62" s="44"/>
+      <c r="M62" s="40"/>
+      <c r="N62" s="14"/>
+      <c r="O62" s="42"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
-      <c r="C63" s="29" t="s">
+      <c r="C63" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="28" t="s">
+      <c r="D63" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E63" s="28"/>
       <c r="F63" s="15"/>
       <c r="G63" s="15"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="M63" s="40"/>
+      <c r="O63" s="42"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="28" t="s">
+      <c r="C64" s="11"/>
+      <c r="D64" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="28"/>
       <c r="F64" s="15"/>
       <c r="G64" s="15"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="M64" s="40"/>
+      <c r="O64" s="42"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D65" s="28" t="s">
+      <c r="D65" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E65" s="28" t="s">
+      <c r="E65" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F65" s="15" t="s">
         <v>27</v>
       </c>
       <c r="G65" s="15"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="M65" s="40"/>
+      <c r="O65" s="42"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="28" t="s">
+      <c r="C66" s="11"/>
+      <c r="D66" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E66" s="28"/>
       <c r="F66" s="15" t="s">
         <v>28</v>
       </c>
       <c r="G66" s="15"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="M66" s="45"/>
+      <c r="O66" s="42"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="28" t="s">
+      <c r="C67" s="11"/>
+      <c r="D67" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E67" s="28"/>
       <c r="F67" s="15" t="s">
         <v>29</v>
       </c>
       <c r="G67" s="15"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="O67" s="42"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="28" t="s">
+      <c r="C68" s="11"/>
+      <c r="D68" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E68" s="28"/>
       <c r="F68" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G68" s="15"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="O68" s="42"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
-      <c r="C69" s="29" t="s">
+      <c r="C69" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
       <c r="F69" s="15" t="s">
         <v>34</v>
       </c>
       <c r="G69" s="15"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="O69" s="44"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="10"/>
       <c r="C70" s="2"/>
@@ -1669,19 +1927,14 @@
       <c r="F70" s="17"/>
       <c r="G70" s="15"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
-      <c r="B71" s="28"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="28"/>
       <c r="G71" s="15"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>2</v>
@@ -1691,105 +1944,90 @@
       <c r="F72" s="8"/>
       <c r="G72" s="15"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
-      <c r="C73" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D73" s="28"/>
-      <c r="E73" s="28"/>
+      <c r="C73" s="11" t="s">
+        <v>60</v>
+      </c>
       <c r="F73" s="15"/>
       <c r="G73" s="15"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="5"/>
-      <c r="C74" s="29" t="s">
+      <c r="C74" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D74" s="28"/>
-      <c r="E74" s="28"/>
       <c r="F74" s="15"/>
       <c r="G74" s="15"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="29" t="s">
+      <c r="C75" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D75" s="28"/>
-      <c r="E75" s="28"/>
       <c r="F75" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G75" s="15"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
       <c r="B76" s="5"/>
-      <c r="C76" s="29" t="s">
+      <c r="C76" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D76" s="28"/>
-      <c r="E76" s="28"/>
       <c r="F76" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G76" s="15"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
-      <c r="C77" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="D77" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="E77" s="28"/>
+      <c r="C77" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="F77" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G77" s="15"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="B78" s="5"/>
-      <c r="C78" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D78" s="28"/>
-      <c r="E78" s="28"/>
+      <c r="C78" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="F78" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G78" s="15"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
-      <c r="C79" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="D79" s="28"/>
-      <c r="E79" s="28"/>
+      <c r="C79" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="F79" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G79" s="15"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
       <c r="B80" s="5"/>
-      <c r="C80" s="29" t="s">
+      <c r="C80" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D80" s="28"/>
-      <c r="E80" s="28"/>
       <c r="F80" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G80" s="15"/>
     </row>
@@ -1797,14 +2035,14 @@
       <c r="A81" s="5"/>
       <c r="B81" s="10"/>
       <c r="C81" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" s="20" t="s">
         <v>66</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E81" s="2"/>
-      <c r="F81" s="30" t="s">
-        <v>68</v>
       </c>
       <c r="G81" s="15"/>
     </row>
@@ -1818,11 +2056,21 @@
       <c r="G82" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="14">
+    <mergeCell ref="M52:M66"/>
+    <mergeCell ref="O52:O69"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="G50:J53"/>
+    <mergeCell ref="L52:L62"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D36:E36"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C13:C15"/>
-    <mergeCell ref="F13:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>